<commit_message>
Update :  journal d'abord Nelson Cuervo
</commit_message>
<xml_diff>
--- a/NelsonCuervo/Sprint3/journal d'abord Nelson Cuervo.xlsx
+++ b/NelsonCuervo/Sprint3/journal d'abord Nelson Cuervo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\DEVELOPPEMENT-APPLICATIOS\projetChantier\NelsonCuervo\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D7D340-CFC0-402B-805B-BED0C54FDD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB3E461-AC78-4D02-8CD6-05C174AC86AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{4E6CA233-FC79-442E-BFA8-A030C94426C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E6CA233-FC79-442E-BFA8-A030C94426C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>Nelson Alfonso Cuervo Caviedes</t>
   </si>
@@ -248,6 +248,13 @@
   </si>
   <si>
     <t>31H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de vidéos explicatives </t>
+  </si>
+  <si>
+    <t xml:space="preserve">réunion avec Leonel pour finaliser les détails de l'application et sa présentation
+</t>
   </si>
 </sst>
 </file>
@@ -295,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -308,8 +315,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -317,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72050F50-CF0C-4E9B-ADE3-1D6CB7D01C36}">
-  <dimension ref="B4:E70"/>
+  <dimension ref="B4:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>7</v>
       </c>
@@ -1393,6 +1403,34 @@
       </c>
       <c r="E70" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="2">
+        <v>52</v>
+      </c>
+      <c r="C71" s="5">
+        <v>44967</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
+        <v>53</v>
+      </c>
+      <c r="C72" s="5">
+        <v>44967</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>